<commit_message>
Implement animation using scripts
</commit_message>
<xml_diff>
--- a/각도 계산.xlsx
+++ b/각도 계산.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>x좌표</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -183,6 +183,22 @@
   </si>
   <si>
     <t>7-&gt;9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-&gt;2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-&gt;3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-&gt;2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-&gt;3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -513,15 +529,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -556,30 +570,47 @@
       </c>
       <c r="F2">
         <f>90-IF(M2&lt;0,K2,L2)</f>
-        <v>153.03032157750462</v>
+        <v>153.03103811712612</v>
       </c>
       <c r="G2">
         <f>IF(F2+180&lt;180,F2+180,F2-180)</f>
-        <v>-26.969678422495377</v>
+        <v>-26.968961882873884</v>
+      </c>
+      <c r="H2">
+        <f>ROUND(F2,0)</f>
+        <v>153</v>
+      </c>
+      <c r="I2">
+        <f>ROUND(G2,0)</f>
+        <v>-27</v>
       </c>
       <c r="J2">
         <f>ATAN(($B$2-$B$4)/($C$2-$C$4))</f>
-        <v>1.1000866401182821</v>
+        <v>1.1000991460938978</v>
       </c>
       <c r="K2">
         <f>-DEGREES(J2)</f>
-        <v>-63.03032157750463</v>
+        <v>-63.031038117126108</v>
       </c>
       <c r="L2">
         <f>IF(180+K2&lt;180,180+K2,"false")</f>
-        <v>116.96967842249538</v>
+        <v>116.96896188287388</v>
       </c>
       <c r="M2">
         <f>$B$2-$B$4</f>
-        <v>-2.3365999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-2.336576</v>
+      </c>
+      <c r="O2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2">
+        <v>63</v>
+      </c>
+      <c r="Q2">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -594,653 +625,958 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F41" si="0">90-IF(M3&lt;0,K3,L3)</f>
-        <v>144.0013282343582</v>
+        <v>144.00134706564575</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G41" si="1">IF(F3+180&lt;180,F3+180,F3-180)</f>
-        <v>-35.998671765641802</v>
+        <v>-35.998652934354254</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:I41" si="2">ROUND(F3,0)</f>
+        <v>144</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="2"/>
+        <v>-36</v>
       </c>
       <c r="J3">
         <f>ATAN((B2-B5)/(C2-C5))</f>
-        <v>0.94250097813972666</v>
+        <v>0.94250130680769695</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K41" si="2">-DEGREES(J3)</f>
-        <v>-54.001328234358198</v>
+        <f t="shared" ref="K3:K41" si="3">-DEGREES(J3)</f>
+        <v>-54.00134706564576</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L5" si="3">IF(180+K3&lt;180,180+K3,"false")</f>
-        <v>125.9986717656418</v>
+        <f t="shared" ref="L3:L5" si="4">IF(180+K3&lt;180,180+K3,"false")</f>
+        <v>125.99865293435424</v>
       </c>
       <c r="M3">
         <f>$B$2-$B$5</f>
-        <v>-2.5529000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-2.5528880000000003</v>
+      </c>
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3">
+        <v>54</v>
+      </c>
+      <c r="Q3">
+        <f>18-144</f>
+        <v>-126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.9865999999999999</v>
+        <v>1.9865759999999999</v>
       </c>
       <c r="C4">
-        <v>2.3889999999999998</v>
+        <v>2.388951</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>117.03078659641898</v>
+        <v>117.03123128090476</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>-62.969213403581023</v>
+        <v>-62.968768719095237</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>-63</v>
       </c>
       <c r="J4">
         <f>ATAN((B2-B6)/(C2-C6))</f>
-        <v>0.47177622551146275</v>
+        <v>0.47178398671987237</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
-        <v>-27.030786596418974</v>
+        <f t="shared" si="3"/>
+        <v>-27.031231280904766</v>
       </c>
       <c r="L4">
-        <f t="shared" si="3"/>
-        <v>152.96921340358102</v>
+        <f t="shared" si="4"/>
+        <v>152.96876871909524</v>
       </c>
       <c r="M4">
         <f>$B$2-$B$6</f>
-        <v>-1.9278</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-1.9278140000000001</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4">
+        <v>27</v>
+      </c>
+      <c r="Q4">
+        <f>-54-117</f>
+        <v>-171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.2029000000000001</v>
+        <v>2.2028880000000002</v>
       </c>
       <c r="C5">
-        <v>3.0547</v>
+        <v>3.0546899999999999</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>108.00147145271809</v>
+        <v>108.00148011337407</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>-71.998528547281907</v>
+        <v>-71.998519886625928</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>-72</v>
       </c>
       <c r="J5">
         <f>ATAN((B2-B7)/(C2-C7))</f>
-        <v>0.31418494705369748</v>
+        <v>0.31418509821065976</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>-18.001471452718093</v>
+        <f t="shared" si="3"/>
+        <v>-18.001480113374079</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
-        <v>161.99852854728192</v>
+        <f t="shared" si="4"/>
+        <v>161.99851988662593</v>
       </c>
       <c r="M5">
         <f>$B$2-$B$7</f>
-        <v>-1.3614999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-1.3615019999999998</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5">
+        <f>108-90</f>
+        <v>18</v>
+      </c>
+      <c r="Q5">
+        <f>-54-108</f>
+        <v>-162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.5778000000000001</v>
+        <v>1.577814</v>
       </c>
       <c r="C6">
-        <v>4.9785000000000004</v>
+        <v>4.9784550000000003</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>81.028216046514203</v>
+        <v>81.028197788021799</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>-98.971783953485797</v>
+        <f>IF(F6+180&lt;180,F6+180,F6-180)+360</f>
+        <v>261.02819778802177</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>261</v>
       </c>
       <c r="J6">
         <f>ATAN((B2-B8)/(C2-C8))</f>
-        <v>-0.15658716976592088</v>
+        <v>-0.1565874884367299</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>8.9717839534857937</v>
+        <f t="shared" si="3"/>
+        <v>8.9718022119782042</v>
       </c>
       <c r="L6">
         <f>IF(180+K6&lt;180,180+K6,K6)</f>
-        <v>8.9717839534857937</v>
+        <v>8.9718022119782042</v>
       </c>
       <c r="M6">
         <f>$B$2-$B$8</f>
-        <v>0.66150000000000009</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+        <v>0.66150199999999992</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6">
+        <v>-9</v>
+      </c>
+      <c r="Q6">
+        <f>234-81</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.0115000000000001</v>
+        <v>1.0115019999999999</v>
       </c>
       <c r="C7">
-        <v>5.3898999999999999</v>
+        <v>5.3899039999999996</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>71.99875287670281</v>
+        <v>71.998360303169932</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>-108.00124712329719</v>
+        <f t="shared" ref="G7:G9" si="5">IF(F7+180&lt;180,F7+180,F7-180)+360</f>
+        <v>251.99836030316993</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>252</v>
       </c>
       <c r="J7">
         <f>ATAN((B2-B9)/(C2-C9))</f>
-        <v>-0.31418103176669371</v>
+        <v>-0.3141878834673984</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
-        <v>18.001247123297198</v>
+        <f t="shared" si="3"/>
+        <v>18.001639696830061</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L41" si="4">IF(180+K7&lt;180,180+K7,K7)</f>
-        <v>18.001247123297198</v>
+        <f t="shared" ref="L7:L41" si="6">IF(180+K7&lt;180,180+K7,K7)</f>
+        <v>18.001639696830061</v>
       </c>
       <c r="M7">
         <f>$B$2-$B$9</f>
-        <v>1.2278000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+        <v>1.227814</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7">
+        <v>-18</v>
+      </c>
+      <c r="Q7">
+        <f>234-72</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-1.0115000000000001</v>
+        <v>-1.0115019999999999</v>
       </c>
       <c r="C8">
-        <v>5.3898999999999999</v>
+        <v>5.3899039999999996</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>45.027816483714744</v>
+        <v>45.027847556154626</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>-134.97218351628527</v>
+        <f t="shared" si="5"/>
+        <v>225.02784755615463</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>225</v>
       </c>
       <c r="J8">
         <f>ATAN((B2-B10)/(C2-C10))</f>
-        <v>-0.78491267417029864</v>
+        <v>-0.78491213185391606</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
-        <v>44.972183516285256</v>
+        <f t="shared" si="3"/>
+        <v>44.972152443845374</v>
       </c>
       <c r="L8">
-        <f t="shared" si="4"/>
-        <v>44.972183516285256</v>
+        <f t="shared" si="6"/>
+        <v>44.972152443845374</v>
       </c>
       <c r="M8">
         <f>$B$2-$B$10</f>
-        <v>1.8529</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+        <v>1.8528880000000001</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8">
+        <v>-45</v>
+      </c>
+      <c r="Q8">
+        <f>162-45</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-1.5778000000000001</v>
+        <v>-1.577814</v>
       </c>
       <c r="C9">
-        <v>4.9785000000000004</v>
+        <v>4.9784550000000003</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>35.998636580244337</v>
+        <v>35.997913293110244</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>-144.00136341975565</v>
+        <f t="shared" si="5"/>
+        <v>215.99791329311023</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>216</v>
       </c>
       <c r="J9">
         <f>ATAN((B2-B11)/(C2-C11))</f>
-        <v>-0.94250159224076102</v>
+        <v>-0.94251421598268825</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
-        <v>54.001363419755663</v>
+        <f t="shared" si="3"/>
+        <v>54.002086706889756</v>
       </c>
       <c r="L9">
-        <f t="shared" si="4"/>
-        <v>54.001363419755663</v>
+        <f t="shared" si="6"/>
+        <v>54.002086706889756</v>
       </c>
       <c r="M9">
         <f>$B$2-$B$11</f>
-        <v>1.6366000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+        <v>1.6365759999999998</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9">
+        <f>36-90</f>
+        <v>-54</v>
+      </c>
+      <c r="Q9">
+        <f>162-36</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-2.2029000000000001</v>
+        <v>-2.2028880000000002</v>
       </c>
       <c r="C10">
-        <v>3.0547</v>
+        <v>3.0546899999999999</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>144.00136341975565</v>
+        <v>144.00208670688977</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>-35.998636580244352</v>
+        <v>-35.99791329311023</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>-36</v>
       </c>
       <c r="J10">
         <f>ATAN((B3-B4)/(C3-C4))</f>
-        <v>0.94250159224076102</v>
+        <v>0.94251421598268825</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
-        <v>-54.001363419755663</v>
+        <f t="shared" si="3"/>
+        <v>-54.002086706889756</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
-        <v>125.99863658024434</v>
+        <f t="shared" si="6"/>
+        <v>125.99791329311024</v>
       </c>
       <c r="M10">
         <f>$B$3-$B$4</f>
-        <v>-1.6366000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-1.6365759999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-1.9865999999999999</v>
+        <v>-1.9865759999999999</v>
       </c>
       <c r="C11">
-        <v>2.3889999999999998</v>
+        <v>2.388951</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>134.97218351628527</v>
+        <v>134.97215244384537</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>-45.02781648371473</v>
+        <v>-45.027847556154626</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>-45</v>
       </c>
       <c r="J11">
         <f>ATAN((B3-B5)/(C3-C5))</f>
-        <v>0.78491267417029864</v>
+        <v>0.78491213185391606</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
-        <v>-44.972183516285256</v>
+        <f t="shared" si="3"/>
+        <v>-44.972152443845374</v>
       </c>
       <c r="L11">
-        <f t="shared" si="4"/>
-        <v>135.02781648371473</v>
+        <f t="shared" si="6"/>
+        <v>135.02784755615463</v>
       </c>
       <c r="M11">
         <f>$B$3-$B$5</f>
-        <v>-1.8529</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-1.8528880000000001</v>
+      </c>
+      <c r="O11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11">
+        <v>54</v>
+      </c>
+      <c r="Q11">
+        <f>18-144</f>
+        <v>-126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E12" t="s">
         <v>28</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>108.00124712329719</v>
+        <v>108.00163969683007</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>-71.99875287670281</v>
+        <v>-71.998360303169932</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>-72</v>
       </c>
       <c r="J12">
         <f>ATAN((B3-B6)/(C3-C6))</f>
-        <v>0.31418103176669371</v>
+        <v>0.3141878834673984</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
-        <v>-18.001247123297198</v>
+        <f t="shared" si="3"/>
+        <v>-18.001639696830061</v>
       </c>
       <c r="L12">
-        <f t="shared" si="4"/>
-        <v>161.99875287670281</v>
+        <f t="shared" si="6"/>
+        <v>161.99836030316993</v>
       </c>
       <c r="M12">
         <f>$B$3-$B$6</f>
-        <v>-1.2278000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-1.227814</v>
+      </c>
+      <c r="O12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12">
+        <v>45</v>
+      </c>
+      <c r="Q12">
+        <v>-117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E13" t="s">
         <v>29</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>98.971783953485797</v>
+        <v>98.971802211978201</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>-81.028216046514203</v>
+        <v>-81.028197788021799</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>-81</v>
       </c>
       <c r="J13">
         <f>ATAN((B3-B7)/(C3-C7))</f>
-        <v>0.15658716976592088</v>
+        <v>0.1565874884367299</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
-        <v>-8.9717839534857937</v>
+        <f t="shared" si="3"/>
+        <v>-8.9718022119782042</v>
       </c>
       <c r="L13">
-        <f t="shared" si="4"/>
-        <v>171.02821604651422</v>
+        <f t="shared" si="6"/>
+        <v>171.0281977880218</v>
       </c>
       <c r="M13">
         <f>$B$3-$B$7</f>
-        <v>-0.66150000000000009</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+        <v>-0.66150199999999992</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13">
+        <v>18</v>
+      </c>
+      <c r="Q13">
+        <v>-162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E14" t="s">
         <v>30</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>71.998528547281907</v>
+        <v>71.998519886625928</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>-108.00147145271809</v>
+        <v>-108.00148011337407</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>-108</v>
       </c>
       <c r="J14">
         <f>ATAN((B3-B8)/(C3-C8))</f>
-        <v>-0.31418494705369748</v>
+        <v>-0.31418509821065976</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
-        <v>18.001471452718093</v>
+        <f t="shared" si="3"/>
+        <v>18.001480113374079</v>
       </c>
       <c r="L14">
-        <f t="shared" si="4"/>
-        <v>18.001471452718093</v>
+        <f t="shared" si="6"/>
+        <v>18.001480113374079</v>
       </c>
       <c r="M14">
         <f>$B$3-$B$8</f>
-        <v>1.3614999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+        <v>1.3615019999999998</v>
+      </c>
+      <c r="O14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14">
+        <v>9</v>
+      </c>
+      <c r="Q14">
+        <v>-153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E15" t="s">
         <v>31</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>62.969213403581023</v>
+        <v>62.968768719095237</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>-117.03078659641898</v>
+        <v>-117.03123128090476</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>-117</v>
       </c>
       <c r="J15">
         <f>ATAN((B3-B9)/(C3-C9))</f>
-        <v>-0.47177622551146275</v>
+        <v>-0.47178398671987237</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
-        <v>27.030786596418974</v>
+        <f t="shared" si="3"/>
+        <v>27.031231280904766</v>
       </c>
       <c r="L15">
-        <f t="shared" si="4"/>
-        <v>27.030786596418974</v>
+        <f t="shared" si="6"/>
+        <v>27.031231280904766</v>
       </c>
       <c r="M15">
         <f>$B$3-$B$9</f>
-        <v>1.9278</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+        <v>1.9278140000000001</v>
+      </c>
+      <c r="O15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15">
+        <v>-18</v>
+      </c>
+      <c r="Q15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E16" t="s">
         <v>32</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>35.998671765641802</v>
+        <v>35.99865293435424</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>-144.0013282343582</v>
+        <v>-144.00134706564575</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>-144</v>
       </c>
       <c r="J16">
         <f>ATAN((B3-B10)/(C3-C10))</f>
-        <v>-0.94250097813972666</v>
+        <v>-0.94250130680769695</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
-        <v>54.001328234358198</v>
+        <f t="shared" si="3"/>
+        <v>54.00134706564576</v>
       </c>
       <c r="L16">
-        <f t="shared" si="4"/>
-        <v>54.001328234358198</v>
+        <f t="shared" si="6"/>
+        <v>54.00134706564576</v>
       </c>
       <c r="M16">
         <f>$B$3-$B$10</f>
-        <v>2.5529000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.4">
+        <v>2.5528880000000003</v>
+      </c>
+      <c r="O16" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16">
+        <v>-27</v>
+      </c>
+      <c r="Q16">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
         <v>33</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>26.96967842249537</v>
+        <v>26.968961882873892</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>-153.03032157750462</v>
+        <v>-153.03103811712612</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>-153</v>
       </c>
       <c r="J17">
         <f>ATAN((B3-B11)/(C3-C11))</f>
-        <v>-1.1000866401182821</v>
+        <v>-1.1000991460938978</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
-        <v>63.03032157750463</v>
+        <f t="shared" si="3"/>
+        <v>63.031038117126108</v>
       </c>
       <c r="L17">
-        <f t="shared" si="4"/>
-        <v>63.03032157750463</v>
+        <f t="shared" si="6"/>
+        <v>63.031038117126108</v>
       </c>
       <c r="M17">
         <f>$B$3-$B11</f>
-        <v>2.3365999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.4">
+        <v>2.336576</v>
+      </c>
+      <c r="O17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17">
+        <v>-54</v>
+      </c>
+      <c r="Q17">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E18" t="s">
         <v>34</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>81.028850464070402</v>
+        <v>81.029684447320136</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>-98.971149535929598</v>
+        <v>-98.970315552679864</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>-99</v>
       </c>
       <c r="J18">
         <f>ATAN((B4-B6)/(C4-C6))</f>
-        <v>-0.15657609709073278</v>
+        <v>-0.15656154133711839</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
-        <v>8.9711495359295963</v>
+        <f t="shared" si="3"/>
+        <v>8.9703155526798586</v>
       </c>
       <c r="L18">
-        <f t="shared" si="4"/>
-        <v>8.9711495359295963</v>
+        <f t="shared" si="6"/>
+        <v>8.9703155526798586</v>
       </c>
       <c r="M18">
         <f>$B$4-$B$6</f>
-        <v>0.40879999999999983</v>
-      </c>
-    </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.4">
+        <v>0.40876199999999985</v>
+      </c>
+      <c r="O18" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18">
+        <v>-63</v>
+      </c>
+      <c r="Q18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E19" t="s">
         <v>35</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>71.999162709178407</v>
+        <v>71.999909114359681</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>-108.00083729082159</v>
+        <v>-108.00009088564032</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>-108</v>
       </c>
       <c r="J19">
         <f>ATAN((B4-B7)/(C4-C7))</f>
-        <v>-0.31417387884061287</v>
+        <v>-0.31416085161264556</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
-        <v>18.000837290821597</v>
+        <f t="shared" si="3"/>
+        <v>18.000090885640315</v>
       </c>
       <c r="L19">
-        <f t="shared" si="4"/>
-        <v>18.000837290821597</v>
+        <f t="shared" si="6"/>
+        <v>18.000090885640315</v>
       </c>
       <c r="M19">
         <f>$B$4-$B$7</f>
-        <v>0.97509999999999986</v>
-      </c>
-    </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.4">
+        <v>0.975074</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>45.026742485578744</v>
+        <v>45.027458660155119</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
-        <v>-134.97325751442125</v>
+        <f>IF(F20+180&lt;180,F20+180,F20-180)+360</f>
+        <v>225.02745866015511</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>225</v>
       </c>
       <c r="J20">
         <f>ATAN((B4-B8)/(C4-C8))</f>
-        <v>-0.78493141897393215</v>
+        <v>-0.78491891936955527</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
-        <v>44.973257514421256</v>
+        <f t="shared" si="3"/>
+        <v>44.972541339844881</v>
       </c>
       <c r="L20">
-        <f t="shared" si="4"/>
-        <v>44.973257514421256</v>
+        <f t="shared" si="6"/>
+        <v>44.972541339844881</v>
       </c>
       <c r="M20">
         <f>$B$4-$B$8</f>
-        <v>2.9981</v>
-      </c>
-    </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.4">
+        <v>2.9980779999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>35.99802006196375</v>
+        <v>35.998138584543675</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>-144.00197993803624</v>
+        <f t="shared" ref="G21:G22" si="7">IF(F21+180&lt;180,F21+180,F21-180)+360</f>
+        <v>215.99813858454368</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>216</v>
       </c>
       <c r="J21">
         <f>ATAN((B4-B9)/(C4-C9))</f>
-        <v>-0.94251235251465593</v>
+        <v>-0.94251028390539837</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
-        <v>54.00197993803625</v>
+        <f t="shared" si="3"/>
+        <v>54.001861415456325</v>
       </c>
       <c r="L21">
-        <f t="shared" si="4"/>
-        <v>54.00197993803625</v>
+        <f t="shared" si="6"/>
+        <v>54.001861415456325</v>
       </c>
       <c r="M21">
         <f>$B$4-$B$9</f>
-        <v>3.5644</v>
-      </c>
-    </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.4">
+        <v>3.5643899999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E22" t="s">
         <v>9</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>9.0286601471018599</v>
+        <v>9.0292566864487753</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>-170.97133985289815</v>
+        <f t="shared" si="7"/>
+        <v>189.02925668644878</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>189</v>
       </c>
       <c r="J22">
         <f>ATAN((B4-B10)/(C4-C10))</f>
-        <v>-1.4132164801843736</v>
+        <v>-1.4132060686086521</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
-        <v>80.97133985289814</v>
+        <f t="shared" si="3"/>
+        <v>80.970743313551225</v>
       </c>
       <c r="L22">
-        <f t="shared" si="4"/>
-        <v>80.97133985289814</v>
+        <f t="shared" si="6"/>
+        <v>80.970743313551225</v>
       </c>
       <c r="M22">
         <f>$B$4-$B$10</f>
-        <v>4.1894999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.4">
+        <v>4.1894640000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E23" t="s">
         <v>10</v>
       </c>
@@ -1249,8 +1585,16 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
-        <v>-180</v>
+        <f>IF(F23+180&lt;180,F23+180,F23-180)+360</f>
+        <v>180</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="J23" t="e">
         <f>ATAN((B4-B11)/(C4-C11))</f>
@@ -1260,131 +1604,163 @@
         <v>90</v>
       </c>
       <c r="L23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="M23">
         <f>$B$4-$B$11</f>
-        <v>3.9731999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.4">
+        <v>3.9731519999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E24" t="s">
         <v>36</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>71.999475011284602</v>
+        <v>71.999869060485906</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>-108.0005249887154</v>
+        <v>-108.00013093951409</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>-108</v>
       </c>
       <c r="J24">
         <f>ATAN((B5-B6)/(C5-C6))</f>
-        <v>-0.31416842814059881</v>
+        <v>-0.31416155068462126</v>
       </c>
       <c r="K24">
-        <f t="shared" si="2"/>
-        <v>18.000524988715398</v>
+        <f t="shared" si="3"/>
+        <v>18.000130939514097</v>
       </c>
       <c r="L24">
-        <f t="shared" si="4"/>
-        <v>18.000524988715398</v>
+        <f t="shared" si="6"/>
+        <v>18.000130939514097</v>
       </c>
       <c r="M24">
         <f>$B$5-$B$6</f>
-        <v>0.62509999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.4">
+        <v>0.62507400000000013</v>
+      </c>
+    </row>
+    <row r="25" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E25" t="s">
         <v>37</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>62.969695972058844</v>
+        <v>62.970107581411106</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>-117.03030402794116</v>
+        <v>-117.0298924185889</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>-117</v>
       </c>
       <c r="J25">
         <f>ATAN((B5-B7)/(C5-C7))</f>
-        <v>-0.47176780310265859</v>
+        <v>-0.47176061916422951</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
-        <v>27.03030402794116</v>
+        <f t="shared" si="3"/>
+        <v>27.029892418588894</v>
       </c>
       <c r="L25">
-        <f t="shared" si="4"/>
-        <v>27.03030402794116</v>
+        <f t="shared" si="6"/>
+        <v>27.029892418588894</v>
       </c>
       <c r="M25">
         <f>$B$5-$B$7</f>
-        <v>1.1914</v>
-      </c>
-    </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.4">
+        <v>1.1913860000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>35.997686455370022</v>
+        <v>35.997934554328467</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>-144.00231354462997</v>
+        <f>IF(F26+180&lt;180,F26+180,F26-180)+360</f>
+        <v>215.99793455432848</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>216</v>
       </c>
       <c r="J26">
         <f>ATAN((B5-B8)/(C5-C8))</f>
-        <v>-0.94251817504812285</v>
+        <v>-0.94251384490442724</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
-        <v>54.002313544629978</v>
+        <f t="shared" si="3"/>
+        <v>54.002065445671533</v>
       </c>
       <c r="L26">
-        <f t="shared" si="4"/>
-        <v>54.002313544629978</v>
+        <f t="shared" si="6"/>
+        <v>54.002065445671533</v>
       </c>
       <c r="M26">
         <f>$B$5-$B$8</f>
-        <v>3.2144000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.4">
+        <v>3.2143899999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>26.969156951432154</v>
+        <v>26.968723373045357</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
-        <v>-153.03084304856785</v>
+        <f t="shared" ref="G27:G28" si="8">IF(F27+180&lt;180,F27+180,F27-180)+360</f>
+        <v>206.96872337304535</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>207</v>
       </c>
       <c r="J27">
         <f>ATAN((B5-B9)/(C5-C9))</f>
-        <v>-1.100095741505289</v>
+        <v>-1.1001033088757042</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
-        <v>63.030843048567846</v>
+        <f t="shared" si="3"/>
+        <v>63.031276626954643</v>
       </c>
       <c r="L27">
-        <f t="shared" si="4"/>
-        <v>63.030843048567846</v>
+        <f t="shared" si="6"/>
+        <v>63.031276626954643</v>
       </c>
       <c r="M27">
         <f>$B$5-$B$9</f>
-        <v>3.7807000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.4">
+        <v>3.7807020000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E28" t="s">
         <v>13</v>
       </c>
@@ -1393,8 +1769,16 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
-        <v>-180</v>
+        <f t="shared" si="8"/>
+        <v>180</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="J28" t="e">
         <f>ATAN((B5-B10)/(C5-C10))</f>
@@ -1404,73 +1788,89 @@
         <v>90</v>
       </c>
       <c r="L28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="M28">
         <f>$B$5-$B$10</f>
-        <v>4.4058000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.4">
+        <v>4.4057760000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E29" t="s">
         <v>14</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>-9.0286601471018599</v>
+        <v>-9.0292566864487753</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>170.97133985289815</v>
+        <v>170.97074331355122</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>171</v>
       </c>
       <c r="J29">
         <f>ATAN((B5-B11)/(C5-C11))</f>
-        <v>1.4132164801843736</v>
+        <v>1.4132060686086521</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
-        <v>-80.97133985289814</v>
+        <f t="shared" si="3"/>
+        <v>-80.970743313551225</v>
       </c>
       <c r="L29">
-        <f t="shared" si="4"/>
-        <v>99.02866014710186</v>
+        <f t="shared" si="6"/>
+        <v>99.029256686448775</v>
       </c>
       <c r="M29">
         <f>$B$5-$B$11</f>
-        <v>4.1894999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.4">
+        <v>4.1894640000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E30" t="s">
         <v>38</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>9.0279558593662728</v>
+        <v>9.0289585525480902</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
-        <v>-170.97204414063373</v>
+        <f>IF(F30+180&lt;180,F30+180,F30-180)+360</f>
+        <v>189.02895855254809</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>189</v>
       </c>
       <c r="J30">
         <f>ATAN((B6-B8)/(C6-C8))</f>
-        <v>-1.4132287723242409</v>
+        <v>-1.4132112720268311</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
-        <v>80.972044140633727</v>
+        <f t="shared" si="3"/>
+        <v>80.97104144745191</v>
       </c>
       <c r="L30">
-        <f t="shared" si="4"/>
-        <v>80.972044140633727</v>
+        <f t="shared" si="6"/>
+        <v>80.97104144745191</v>
       </c>
       <c r="M30">
         <f>$B$6-$B$8</f>
-        <v>2.5893000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.4">
+        <v>2.5893160000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E31" t="s">
         <v>39</v>
       </c>
@@ -1479,8 +1879,16 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>-180</v>
+        <f>IF(F31+180&lt;180,F31+180,F31-180)+360</f>
+        <v>180</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="J31" t="e">
         <f>ATAN((B6-B9)/(C6-C9))</f>
@@ -1490,41 +1898,49 @@
         <v>90</v>
       </c>
       <c r="L31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="M31">
         <f>$B$6-$B$9</f>
-        <v>3.1556000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.4">
+        <v>3.1556280000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="5:17" x14ac:dyDescent="0.4">
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>-26.969156951432154</v>
+        <v>-26.96872337304535</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>153.03084304856785</v>
+        <v>153.03127662695465</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>-27</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>153</v>
       </c>
       <c r="J32">
         <f>ATAN((B6-B10)/(C6-C10))</f>
-        <v>1.100095741505289</v>
+        <v>1.1001033088757042</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
-        <v>-63.030843048567846</v>
+        <f t="shared" si="3"/>
+        <v>-63.031276626954643</v>
       </c>
       <c r="L32">
-        <f t="shared" si="4"/>
-        <v>116.96915695143215</v>
+        <f t="shared" si="6"/>
+        <v>116.96872337304535</v>
       </c>
       <c r="M32">
         <f>$B$6-$B$10</f>
-        <v>3.7807000000000004</v>
+        <v>3.7807020000000002</v>
       </c>
     </row>
     <row r="33" spans="5:13" x14ac:dyDescent="0.4">
@@ -1533,27 +1949,35 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>-35.998020061963757</v>
+        <v>-35.998138584543682</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>144.00197993803624</v>
+        <v>144.00186141545632</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>-36</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>144</v>
       </c>
       <c r="J33">
         <f>ATAN((B6-B11)/(C6-C11))</f>
-        <v>0.94251235251465593</v>
+        <v>0.94251028390539837</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
-        <v>-54.00197993803625</v>
+        <f t="shared" si="3"/>
+        <v>-54.001861415456325</v>
       </c>
       <c r="L33">
-        <f t="shared" si="4"/>
-        <v>125.99802006196376</v>
+        <f t="shared" si="6"/>
+        <v>125.99813858454368</v>
       </c>
       <c r="M33">
         <f>$B$6-$B$11</f>
-        <v>3.5644</v>
+        <v>3.5643899999999999</v>
       </c>
     </row>
     <row r="34" spans="5:13" x14ac:dyDescent="0.4">
@@ -1565,8 +1989,16 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
-        <v>-180</v>
+        <f>IF(F34+180&lt;180,F34+180,F34-180)+360</f>
+        <v>180</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="J34" t="e">
         <f>ATAN((B7-B8)/(C7-C8))</f>
@@ -1576,12 +2008,12 @@
         <v>90</v>
       </c>
       <c r="L34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="M34">
         <f>$B$7-$B$8</f>
-        <v>2.0230000000000001</v>
+        <v>2.0230039999999998</v>
       </c>
     </row>
     <row r="35" spans="5:13" x14ac:dyDescent="0.4">
@@ -1590,27 +2022,35 @@
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>-9.0279558593662728</v>
+        <v>-9.0289585525480902</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>170.97204414063373</v>
+        <v>170.97104144745191</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>171</v>
       </c>
       <c r="J35">
         <f>ATAN((B7-B9)/(C7-C9))</f>
-        <v>1.4132287723242409</v>
+        <v>1.4132112720268311</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
-        <v>-80.972044140633727</v>
+        <f t="shared" si="3"/>
+        <v>-80.97104144745191</v>
       </c>
       <c r="L35">
-        <f t="shared" si="4"/>
-        <v>99.027955859366273</v>
+        <f t="shared" si="6"/>
+        <v>99.02895855254809</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35" si="5">$B$7-$B$9</f>
-        <v>2.5893000000000002</v>
+        <f t="shared" ref="M35" si="9">$B$7-$B$9</f>
+        <v>2.5893160000000002</v>
       </c>
     </row>
     <row r="36" spans="5:13" x14ac:dyDescent="0.4">
@@ -1619,27 +2059,35 @@
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>-35.99768645537003</v>
+        <v>-35.997934554328467</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>144.00231354462997</v>
+        <v>144.00206544567152</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>-36</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>144</v>
       </c>
       <c r="J36">
         <f>ATAN((B7-B10)/(C7-C10))</f>
-        <v>0.94251817504812285</v>
+        <v>0.94251384490442724</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
-        <v>-54.002313544629978</v>
+        <f t="shared" si="3"/>
+        <v>-54.002065445671533</v>
       </c>
       <c r="L36">
-        <f t="shared" si="4"/>
-        <v>125.99768645537003</v>
+        <f t="shared" si="6"/>
+        <v>125.99793455432847</v>
       </c>
       <c r="M36">
         <f>$B$7-$B$10</f>
-        <v>3.2144000000000004</v>
+        <v>3.2143899999999999</v>
       </c>
     </row>
     <row r="37" spans="5:13" x14ac:dyDescent="0.4">
@@ -1648,27 +2096,35 @@
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>-45.026742485578751</v>
+        <v>-45.027458660155105</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>134.97325751442125</v>
+        <v>134.97254133984489</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>-45</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="J37">
         <f>ATAN((B7-B11)/(C7-C11))</f>
-        <v>0.78493141897393215</v>
+        <v>0.78491891936955527</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
-        <v>-44.973257514421256</v>
+        <f t="shared" si="3"/>
+        <v>-44.972541339844881</v>
       </c>
       <c r="L37">
-        <f t="shared" si="4"/>
-        <v>135.02674248557875</v>
+        <f t="shared" si="6"/>
+        <v>135.02745866015511</v>
       </c>
       <c r="M37">
         <f>$B$7-$B$11</f>
-        <v>2.9981</v>
+        <v>2.9980779999999996</v>
       </c>
     </row>
     <row r="38" spans="5:13" x14ac:dyDescent="0.4">
@@ -1676,28 +2132,36 @@
         <v>42</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
-        <v>-62.969695972058844</v>
+        <f>90-IF(M38&lt;0,K38,L38)+360</f>
+        <v>297.02989241858893</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>117.03030402794116</v>
+        <v>117.02989241858893</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>297</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>117</v>
       </c>
       <c r="J38">
         <f>ATAN((B8-B10)/(C8-C10))</f>
-        <v>0.47176780310265859</v>
+        <v>0.47176061916422951</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
-        <v>-27.03030402794116</v>
+        <f t="shared" si="3"/>
+        <v>-27.029892418588894</v>
       </c>
       <c r="L38">
-        <f t="shared" si="4"/>
-        <v>152.96969597205884</v>
+        <f t="shared" si="6"/>
+        <v>152.9701075814111</v>
       </c>
       <c r="M38">
         <f>$B$8-$B$10</f>
-        <v>1.1914</v>
+        <v>1.1913860000000003</v>
       </c>
     </row>
     <row r="39" spans="5:13" x14ac:dyDescent="0.4">
@@ -1705,28 +2169,36 @@
         <v>43</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
-        <v>-71.999162709178393</v>
+        <f t="shared" ref="F39:F41" si="10">90-IF(M39&lt;0,K39,L39)+360</f>
+        <v>288.0000908856403</v>
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>108.00083729082161</v>
+        <v>108.0000908856403</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>108</v>
       </c>
       <c r="J39">
         <f>ATAN((B8-B11)/(C8-C11))</f>
-        <v>0.31417387884061287</v>
+        <v>0.31416085161264556</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
-        <v>-18.000837290821597</v>
+        <f t="shared" si="3"/>
+        <v>-18.000090885640315</v>
       </c>
       <c r="L39">
-        <f t="shared" si="4"/>
-        <v>161.99916270917839</v>
+        <f t="shared" si="6"/>
+        <v>161.9999091143597</v>
       </c>
       <c r="M39">
         <f>$B$8-$B$11</f>
-        <v>0.97509999999999986</v>
+        <v>0.975074</v>
       </c>
     </row>
     <row r="40" spans="5:13" x14ac:dyDescent="0.4">
@@ -1734,28 +2206,36 @@
         <v>44</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
-        <v>-71.999475011284602</v>
+        <f t="shared" si="10"/>
+        <v>288.00013093951407</v>
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>108.0005249887154</v>
+        <v>108.00013093951407</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>108</v>
       </c>
       <c r="J40">
         <f>ATAN((B9-B10)/(C9-C10))</f>
-        <v>0.31416842814059881</v>
+        <v>0.31416155068462126</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
-        <v>-18.000524988715398</v>
+        <f t="shared" si="3"/>
+        <v>-18.000130939514097</v>
       </c>
       <c r="L40">
-        <f t="shared" si="4"/>
-        <v>161.9994750112846</v>
+        <f t="shared" si="6"/>
+        <v>161.99986906048591</v>
       </c>
       <c r="M40">
         <f>$B$9-$B$10</f>
-        <v>0.62509999999999999</v>
+        <v>0.62507400000000013</v>
       </c>
     </row>
     <row r="41" spans="5:13" x14ac:dyDescent="0.4">
@@ -1763,28 +2243,36 @@
         <v>45</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
-        <v>-81.028850464070416</v>
+        <f t="shared" si="10"/>
+        <v>278.97031555267984</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>98.971149535929584</v>
+        <v>98.970315552679835</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>99</v>
       </c>
       <c r="J41">
         <f>ATAN((B9-B11)/(C9-C11))</f>
-        <v>0.15657609709073278</v>
+        <v>0.15656154133711839</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
-        <v>-8.9711495359295963</v>
+        <f t="shared" si="3"/>
+        <v>-8.9703155526798586</v>
       </c>
       <c r="L41">
-        <f t="shared" si="4"/>
-        <v>171.02885046407042</v>
+        <f t="shared" si="6"/>
+        <v>171.02968444732014</v>
       </c>
       <c r="M41">
         <f>$B$89-$B$11</f>
-        <v>1.9865999999999999</v>
+        <v>1.9865759999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>